<commit_message>
Adaugare Teste server + comentarii
</commit_message>
<xml_diff>
--- a/test_cases_summary.xlsx
+++ b/test_cases_summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agavr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agavr\Desktop\Dosar Ip\Proiect-IP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8B97F3-8250-4744-BE4F-A2BD40D79C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208AF6A5-04C8-4F95-BE4E-E22B1D6C627F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="156">
   <si>
     <t>Nr. caz test</t>
   </si>
@@ -332,6 +332,162 @@
   </si>
   <si>
     <t>CautareDoarIntarziati</t>
+  </si>
+  <si>
+    <t>username=existingUser, password=correctHash, role=bibliotecar</t>
+  </si>
+  <si>
+    <t>Login successful.</t>
+  </si>
+  <si>
+    <t>username=nonexistent, password=wrong, role=bibliotecar</t>
+  </si>
+  <si>
+    <t>Login failed. Invalid data.</t>
+  </si>
+  <si>
+    <t>Two consecutive logins with username=existingUser, password=correctHash, role=bibliotecar</t>
+  </si>
+  <si>
+    <t>First login: Login successful., Second login: Login failed.</t>
+  </si>
+  <si>
+    <t>RegisterSubscriber</t>
+  </si>
+  <si>
+    <t>nume=TestSub, prenume=User, adresa=Some Address, telefon=&lt;unique&gt;, email=testsub@example.com</t>
+  </si>
+  <si>
+    <t>Subscriber Register successful.</t>
+  </si>
+  <si>
+    <t>nume=Already, prenume=Exists, adresa=Any, telefon=0700111222, email=dup@example.com</t>
+  </si>
+  <si>
+    <t>Subscriber registration failed.</t>
+  </si>
+  <si>
+    <t>LoginSubscriber</t>
+  </si>
+  <si>
+    <t>username=0700765432</t>
+  </si>
+  <si>
+    <t>Subscriber Login successful|&lt;id&gt;|&lt;status&gt;|...</t>
+  </si>
+  <si>
+    <t>username=0000000000</t>
+  </si>
+  <si>
+    <t>Subscriber Login failed</t>
+  </si>
+  <si>
+    <t>SearchBooks</t>
+  </si>
+  <si>
+    <t>title=ZZZNonexistentTitle, author=Nobody</t>
+  </si>
+  <si>
+    <t>No books found.</t>
+  </si>
+  <si>
+    <t>title=Alpha, author=AuthorMatch</t>
+  </si>
+  <si>
+    <t>List of matching books in format id~title~author|...</t>
+  </si>
+  <si>
+    <t>subscriberId=-1, bookId=-1, selectedLocation=acasa</t>
+  </si>
+  <si>
+    <t>Inserted Loan failed.</t>
+  </si>
+  <si>
+    <t>subscriberId=&lt;valid&gt;, bookId=&lt;valid&gt;, selectedLocation=acasa</t>
+  </si>
+  <si>
+    <t>Inserted Loan successful.</t>
+  </si>
+  <si>
+    <t>GetLoans</t>
+  </si>
+  <si>
+    <t>subscriberId=-1</t>
+  </si>
+  <si>
+    <t>No loans found.</t>
+  </si>
+  <si>
+    <t>subscriberId=-1, bookId=-1</t>
+  </si>
+  <si>
+    <t>Book return failed.</t>
+  </si>
+  <si>
+    <t>GetStatusClient</t>
+  </si>
+  <si>
+    <t>subcriberId=-1</t>
+  </si>
+  <si>
+    <t>Status not found.</t>
+  </si>
+  <si>
+    <t>RegisterEmployee</t>
+  </si>
+  <si>
+    <t>username=tempEmp, password=pw, role=nonexistentRole</t>
+  </si>
+  <si>
+    <t>Employee registration failed.</t>
+  </si>
+  <si>
+    <t>DeleteLibrarian</t>
+  </si>
+  <si>
+    <t>username=noSuchUser</t>
+  </si>
+  <si>
+    <t>Librarian deletion failed.</t>
+  </si>
+  <si>
+    <t>AddBook</t>
+  </si>
+  <si>
+    <t>isbn=INVALIDISBN, title=null, author=A, genre=G, publisher=P</t>
+  </si>
+  <si>
+    <t>SearchBook</t>
+  </si>
+  <si>
+    <t>isbn=0000000000</t>
+  </si>
+  <si>
+    <t>No books found with the given ISBN.</t>
+  </si>
+  <si>
+    <t>idBook=-9999</t>
+  </si>
+  <si>
+    <t>Book deletion failed.</t>
+  </si>
+  <si>
+    <t>SearchSubscribers</t>
+  </si>
+  <si>
+    <t>no parameters</t>
+  </si>
+  <si>
+    <t>No subscribers found with restrictions or blocked.</t>
+  </si>
+  <si>
+    <t>UpdateStatus</t>
+  </si>
+  <si>
+    <t>subscriberId=-1, status=cu restrictii</t>
+  </si>
+  <si>
+    <t>Status update failed.</t>
   </si>
 </sst>
 </file>
@@ -699,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1694,6 +1850,426 @@
         <v>81</v>
       </c>
     </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" t="s">
+        <v>105</v>
+      </c>
+      <c r="E50" t="s">
+        <v>105</v>
+      </c>
+      <c r="F50" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" t="s">
+        <v>107</v>
+      </c>
+      <c r="F51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" t="s">
+        <v>109</v>
+      </c>
+      <c r="E52" t="s">
+        <v>109</v>
+      </c>
+      <c r="F52" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" t="s">
+        <v>111</v>
+      </c>
+      <c r="D53" t="s">
+        <v>112</v>
+      </c>
+      <c r="E53" t="s">
+        <v>112</v>
+      </c>
+      <c r="F53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" t="s">
+        <v>114</v>
+      </c>
+      <c r="E54" t="s">
+        <v>114</v>
+      </c>
+      <c r="F54" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>115</v>
+      </c>
+      <c r="C55" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" t="s">
+        <v>117</v>
+      </c>
+      <c r="E55" t="s">
+        <v>117</v>
+      </c>
+      <c r="F55" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" t="s">
+        <v>118</v>
+      </c>
+      <c r="D56" t="s">
+        <v>119</v>
+      </c>
+      <c r="E56" t="s">
+        <v>119</v>
+      </c>
+      <c r="F56" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>120</v>
+      </c>
+      <c r="C57" t="s">
+        <v>121</v>
+      </c>
+      <c r="D57" t="s">
+        <v>122</v>
+      </c>
+      <c r="E57" t="s">
+        <v>122</v>
+      </c>
+      <c r="F57" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" t="s">
+        <v>123</v>
+      </c>
+      <c r="D58" t="s">
+        <v>124</v>
+      </c>
+      <c r="E58" t="s">
+        <v>124</v>
+      </c>
+      <c r="F58" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>87</v>
+      </c>
+      <c r="C59" t="s">
+        <v>125</v>
+      </c>
+      <c r="D59" t="s">
+        <v>126</v>
+      </c>
+      <c r="E59" t="s">
+        <v>126</v>
+      </c>
+      <c r="F59" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" t="s">
+        <v>127</v>
+      </c>
+      <c r="D60" t="s">
+        <v>128</v>
+      </c>
+      <c r="E60" t="s">
+        <v>128</v>
+      </c>
+      <c r="F60" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>129</v>
+      </c>
+      <c r="C61" t="s">
+        <v>130</v>
+      </c>
+      <c r="D61" t="s">
+        <v>131</v>
+      </c>
+      <c r="E61" t="s">
+        <v>131</v>
+      </c>
+      <c r="F61" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" t="s">
+        <v>132</v>
+      </c>
+      <c r="D62" t="s">
+        <v>133</v>
+      </c>
+      <c r="E62" t="s">
+        <v>133</v>
+      </c>
+      <c r="F62" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>134</v>
+      </c>
+      <c r="C63" t="s">
+        <v>135</v>
+      </c>
+      <c r="D63" t="s">
+        <v>136</v>
+      </c>
+      <c r="E63" t="s">
+        <v>136</v>
+      </c>
+      <c r="F63" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>137</v>
+      </c>
+      <c r="C64" t="s">
+        <v>138</v>
+      </c>
+      <c r="D64" t="s">
+        <v>139</v>
+      </c>
+      <c r="E64" t="s">
+        <v>139</v>
+      </c>
+      <c r="F64" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>140</v>
+      </c>
+      <c r="C65" t="s">
+        <v>141</v>
+      </c>
+      <c r="D65" t="s">
+        <v>142</v>
+      </c>
+      <c r="E65" t="s">
+        <v>142</v>
+      </c>
+      <c r="F65" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>143</v>
+      </c>
+      <c r="C66" t="s">
+        <v>144</v>
+      </c>
+      <c r="D66" t="s">
+        <v>77</v>
+      </c>
+      <c r="E66" t="s">
+        <v>77</v>
+      </c>
+      <c r="F66" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>145</v>
+      </c>
+      <c r="C67" t="s">
+        <v>146</v>
+      </c>
+      <c r="D67" t="s">
+        <v>147</v>
+      </c>
+      <c r="E67" t="s">
+        <v>147</v>
+      </c>
+      <c r="F67" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>90</v>
+      </c>
+      <c r="C68" t="s">
+        <v>148</v>
+      </c>
+      <c r="D68" t="s">
+        <v>149</v>
+      </c>
+      <c r="E68" t="s">
+        <v>149</v>
+      </c>
+      <c r="F68" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>150</v>
+      </c>
+      <c r="C69" t="s">
+        <v>151</v>
+      </c>
+      <c r="D69" t="s">
+        <v>152</v>
+      </c>
+      <c r="E69" t="s">
+        <v>152</v>
+      </c>
+      <c r="F69" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>153</v>
+      </c>
+      <c r="C70" t="s">
+        <v>154</v>
+      </c>
+      <c r="D70" t="s">
+        <v>155</v>
+      </c>
+      <c r="E70" t="s">
+        <v>155</v>
+      </c>
+      <c r="F70" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>